<commit_message>
revisi dropdown tata naskah
</commit_message>
<xml_diff>
--- a/public/template/2. template peraturan.xlsx
+++ b/public/template/2. template peraturan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/sesendokneo/public/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alwi_mansyur/htdocs/sesendokneo/public/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859466D3-C766-F143-BF0D-6C7EA57D791A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83346F0D-1E27-0D40-AEA3-B5E540E0BD07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="25700" windowHeight="20000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="peraturan" sheetId="1" r:id="rId1"/>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Type Dok</t>
   </si>
@@ -219,6 +219,21 @@
   </si>
   <si>
     <t>KEPUTUSAN MENTERI DALAM NEGERI Nomor 050-5889 TAHUN 2021</t>
+  </si>
+  <si>
+    <t>5 TAHUN 2021</t>
+  </si>
+  <si>
+    <t>PERATURAN ARSIP NASIONAL REPUBLIK INDONESIA</t>
+  </si>
+  <si>
+    <t>PEDOMAN UMUM TATA NASKAH DINAS</t>
+  </si>
+  <si>
+    <t>BERITA NEGARA REPUBLIK INDONESIA TAHUN 2021 NOMOR 758</t>
+  </si>
+  <si>
+    <t>peraturan lembaga</t>
   </si>
 </sst>
 </file>
@@ -1557,13 +1572,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1734,6 +1749,38 @@
         <v>17</v>
       </c>
     </row>
+    <row r="6" spans="1:10" ht="68.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="8">
+        <v>44372</v>
+      </c>
+      <c r="H6" s="8">
+        <v>44372</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>

</xml_diff>